<commit_message>
New version by Apoorva
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\Fidelity\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7755"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Req. No</t>
   </si>
@@ -614,7 +609,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -622,11 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1059,26 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>

</xml_diff>